<commit_message>
Updates to curtailment function and transmission elasticity
</commit_message>
<xml_diff>
--- a/InputData/elec/EoTCCwTC/Elasticity of TCC wrt Transmission Capacity.xlsx
+++ b/InputData/elec/EoTCCwTC/Elasticity of TCC wrt Transmission Capacity.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\EoTCCwTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\elec\EoTCCwTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AECC774-7DB1-4B1A-8EB3-A1110549F1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="19418" windowHeight="10418"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Order2" hidden="1">255</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,6 +35,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -359,7 +362,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -776,24 +779,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="124.46484375" customWidth="1"/>
+    <col min="2" max="2" width="124.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
@@ -801,144 +804,144 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="17">
         <v>2013</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="17">
         <v>2015</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -946,16 +949,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -963,7 +966,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -971,7 +974,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -979,7 +982,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -987,7 +990,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -995,7 +998,7 @@
         <v>2573</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>2598</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>2598</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>14</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>17</v>
       </c>
@@ -1035,7 +1038,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>18</v>
       </c>
@@ -1043,7 +1046,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>19</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20</v>
       </c>
@@ -1059,7 +1062,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>22</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>23</v>
       </c>
@@ -1075,7 +1078,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>27</v>
       </c>
@@ -1083,7 +1086,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>29</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>30</v>
       </c>
@@ -1099,7 +1102,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>31</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>35</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>36</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>42</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>46</v>
       </c>
@@ -1139,7 +1142,7 @@
         <v>10623</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>47</v>
       </c>
@@ -1147,7 +1150,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>48</v>
       </c>
@@ -1155,7 +1158,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>49</v>
       </c>
@@ -1163,7 +1166,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>50</v>
       </c>
@@ -1171,7 +1174,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>51</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>52</v>
       </c>
@@ -1187,7 +1190,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>60</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>61</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>65</v>
       </c>
@@ -1211,7 +1214,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>66</v>
       </c>
@@ -1219,7 +1222,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>75</v>
       </c>
@@ -1227,7 +1230,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>76</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>78</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>80</v>
       </c>
@@ -1257,25 +1260,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AP19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.46484375" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>94</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1291,7 +1294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>95</v>
       </c>
@@ -1337,7 +1340,7 @@
       <c r="AO5" s="7"/>
       <c r="AP5" s="7"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2010</v>
       </c>
@@ -1462,7 +1465,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1590,13 +1593,13 @@
         <v>180319148.93617034</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>72.557000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1614,7 +1617,7 @@
         <v>72.777370539104041</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1623,7 +1626,7 @@
         <v>74.705612756264287</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
@@ -1631,7 +1634,7 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:42" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:42" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -1642,7 +1645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>7.8E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -1672,7 +1675,7 @@
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -1687,7 +1690,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -1706,29 +1709,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AH225"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A160" sqref="A160:AH176"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.1328125" customWidth="1"/>
+    <col min="1" max="1" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>84</v>
       </c>
@@ -1736,12 +1739,12 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="6" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>611.19000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>309.89800000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -2157,7 +2160,7 @@
         <v>896.66899999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -2261,7 +2264,7 @@
         <v>691.34500000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>1777.89</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2469,7 +2472,7 @@
         <v>523.17200000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -2573,7 +2576,7 @@
         <v>97.863</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -2677,7 +2680,7 @@
         <v>1.9299600000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>70.645200000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -2885,7 +2888,7 @@
         <v>13.777900000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -2989,7 +2992,7 @@
         <v>129.67099999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -3093,7 +3096,7 @@
         <v>24.215399999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -3197,7 +3200,7 @@
         <v>197.87200000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -3301,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -3405,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -3509,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -3518,7 +3521,7 @@
         <v>0.36970138543268172</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -3527,7 +3530,7 @@
         <v>0.11620706335185386</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -3631,7 +3634,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -3735,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -3839,7 +3842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -3943,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -4047,7 +4050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -4151,7 +4154,7 @@
         <v>353924000</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -4255,7 +4258,7 @@
         <v>52237800</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -4359,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -4463,7 +4466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -4567,7 +4570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -4671,7 +4674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -4775,7 +4778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -4879,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -4983,7 +4986,7 @@
         <v>62686.9</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -5087,7 +5090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -5191,7 +5194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -5295,7 +5298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -5304,7 +5307,7 @@
         <v>0.17916463971875152</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -5313,7 +5316,7 @@
         <v>8.4114099849444859E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>71</v>
       </c>
@@ -5322,12 +5325,12 @@
         <v>0.15643290056943229</v>
       </c>
     </row>
-    <row r="50" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -5431,7 +5434,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -5535,7 +5538,7 @@
         <v>650.79399999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -5639,7 +5642,7 @@
         <v>342.49900000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -5743,7 +5746,7 @@
         <v>813.875</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -5847,7 +5850,7 @@
         <v>684.15700000000004</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>39</v>
       </c>
@@ -5951,7 +5954,7 @@
         <v>1893.47</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>40</v>
       </c>
@@ -6055,7 +6058,7 @@
         <v>522.32500000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>41</v>
       </c>
@@ -6159,7 +6162,7 @@
         <v>96.190399999999997</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -6263,7 +6266,7 @@
         <v>2.1644699999999999E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -6367,7 +6370,7 @@
         <v>70.859099999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>44</v>
       </c>
@@ -6471,7 +6474,7 @@
         <v>13.777900000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>45</v>
       </c>
@@ -6575,7 +6578,7 @@
         <v>129.67099999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>46</v>
       </c>
@@ -6679,7 +6682,7 @@
         <v>27.408899999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>47</v>
       </c>
@@ -6783,7 +6786,7 @@
         <v>114.91200000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -6887,7 +6890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>49</v>
       </c>
@@ -6991,7 +6994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>50</v>
       </c>
@@ -7095,7 +7098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>51</v>
       </c>
@@ -7104,7 +7107,7 @@
         <v>0.37470222637936812</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>52</v>
       </c>
@@ -7113,7 +7116,7 @@
         <v>0.11539592439581982</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>34</v>
       </c>
@@ -7217,7 +7220,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>53</v>
       </c>
@@ -7321,7 +7324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>54</v>
       </c>
@@ -7425,7 +7428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>55</v>
       </c>
@@ -7529,7 +7532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>56</v>
       </c>
@@ -7633,7 +7636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>57</v>
       </c>
@@ -7737,7 +7740,7 @@
         <v>181611000</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>58</v>
       </c>
@@ -7841,7 +7844,7 @@
         <v>26685900</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>59</v>
       </c>
@@ -7945,7 +7948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>60</v>
       </c>
@@ -8049,7 +8052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>61</v>
       </c>
@@ -8153,7 +8156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>62</v>
       </c>
@@ -8257,7 +8260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>63</v>
       </c>
@@ -8361,7 +8364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>64</v>
       </c>
@@ -8465,7 +8468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>65</v>
       </c>
@@ -8569,7 +8572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>66</v>
       </c>
@@ -8673,7 +8676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>67</v>
       </c>
@@ -8777,7 +8780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>68</v>
       </c>
@@ -8881,7 +8884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>69</v>
       </c>
@@ -8890,7 +8893,7 @@
         <v>9.0426522444435373E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>70</v>
       </c>
@@ -8899,7 +8902,7 @@
         <v>4.3145085797378691E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>71</v>
       </c>
@@ -8908,12 +8911,12 @@
         <v>7.9293884869656495E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>34</v>
       </c>
@@ -9017,7 +9020,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="96" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>35</v>
       </c>
@@ -9121,7 +9124,7 @@
         <v>675.56700000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>36</v>
       </c>
@@ -9225,7 +9228,7 @@
         <v>363.95499999999998</v>
       </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>37</v>
       </c>
@@ -9329,7 +9332,7 @@
         <v>795.476</v>
       </c>
     </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>38</v>
       </c>
@@ -9433,7 +9436,7 @@
         <v>679.53200000000004</v>
       </c>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>39</v>
       </c>
@@ -9537,7 +9540,7 @@
         <v>1898.14</v>
       </c>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>40</v>
       </c>
@@ -9641,7 +9644,7 @@
         <v>523.30200000000002</v>
       </c>
     </row>
-    <row r="102" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>41</v>
       </c>
@@ -9745,7 +9748,7 @@
         <v>95.353999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>42</v>
       </c>
@@ -9849,7 +9852,7 @@
         <v>2.3176099999999999E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>43</v>
       </c>
@@ -9953,7 +9956,7 @@
         <v>70.930400000000006</v>
       </c>
     </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>44</v>
       </c>
@@ -10057,7 +10060,7 @@
         <v>13.777900000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>45</v>
       </c>
@@ -10161,7 +10164,7 @@
         <v>129.67099999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>46</v>
       </c>
@@ -10265,7 +10268,7 @@
         <v>29.797899999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>47</v>
       </c>
@@ -10369,7 +10372,7 @@
         <v>86.616799999999998</v>
       </c>
     </row>
-    <row r="109" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -10473,7 +10476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>49</v>
       </c>
@@ -10577,7 +10580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>50</v>
       </c>
@@ -10681,7 +10684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>51</v>
       </c>
@@ -10690,7 +10693,7 @@
         <v>0.37014388752038835</v>
       </c>
     </row>
-    <row r="114" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>52</v>
       </c>
@@ -10699,7 +10702,7 @@
         <v>0.1153752121558739</v>
       </c>
     </row>
-    <row r="116" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>34</v>
       </c>
@@ -10803,7 +10806,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>53</v>
       </c>
@@ -10907,7 +10910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>54</v>
       </c>
@@ -11011,7 +11014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>55</v>
       </c>
@@ -11115,7 +11118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>56</v>
       </c>
@@ -11219,7 +11222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>57</v>
       </c>
@@ -11323,7 +11326,7 @@
         <v>120947000</v>
       </c>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>58</v>
       </c>
@@ -11427,7 +11430,7 @@
         <v>18832700</v>
       </c>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>59</v>
       </c>
@@ -11531,7 +11534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>60</v>
       </c>
@@ -11635,7 +11638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>61</v>
       </c>
@@ -11739,7 +11742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>62</v>
       </c>
@@ -11843,7 +11846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>63</v>
       </c>
@@ -11947,7 +11950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>64</v>
       </c>
@@ -12051,7 +12054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>65</v>
       </c>
@@ -12155,7 +12158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>66</v>
       </c>
@@ -12259,7 +12262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>67</v>
       </c>
@@ -12363,7 +12366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>68</v>
       </c>
@@ -12467,7 +12470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>69</v>
       </c>
@@ -12476,7 +12479,7 @@
         <v>6.0937944638859529E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>70</v>
       </c>
@@ -12485,7 +12488,7 @@
         <v>3.0441311488129098E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>71</v>
       </c>
@@ -12494,12 +12497,12 @@
         <v>5.3690947513202678E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="139" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>34</v>
       </c>
@@ -12603,7 +12606,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="140" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>35</v>
       </c>
@@ -12707,7 +12710,7 @@
         <v>661.98099999999999</v>
       </c>
     </row>
-    <row r="141" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>36</v>
       </c>
@@ -12811,7 +12814,7 @@
         <v>350.93200000000002</v>
       </c>
     </row>
-    <row r="142" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>37</v>
       </c>
@@ -12915,7 +12918,7 @@
         <v>795.476</v>
       </c>
     </row>
-    <row r="143" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>38</v>
       </c>
@@ -13019,7 +13022,7 @@
         <v>679.66899999999998</v>
       </c>
     </row>
-    <row r="144" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>39</v>
       </c>
@@ -13123,7 +13126,7 @@
         <v>1918.66</v>
       </c>
     </row>
-    <row r="145" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>40</v>
       </c>
@@ -13227,7 +13230,7 @@
         <v>528.88499999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>41</v>
       </c>
@@ -13331,7 +13334,7 @@
         <v>95.353999999999999</v>
       </c>
     </row>
-    <row r="147" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>42</v>
       </c>
@@ -13435,7 +13438,7 @@
         <v>2.2325800000000001E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>43</v>
       </c>
@@ -13539,7 +13542,7 @@
         <v>70.930400000000006</v>
       </c>
     </row>
-    <row r="149" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>44</v>
       </c>
@@ -13643,7 +13646,7 @@
         <v>13.777900000000001</v>
       </c>
     </row>
-    <row r="150" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>45</v>
       </c>
@@ -13747,7 +13750,7 @@
         <v>129.67099999999999</v>
       </c>
     </row>
-    <row r="151" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>46</v>
       </c>
@@ -13851,7 +13854,7 @@
         <v>28.921800000000001</v>
       </c>
     </row>
-    <row r="152" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>47</v>
       </c>
@@ -13955,7 +13958,7 @@
         <v>87.032899999999998</v>
       </c>
     </row>
-    <row r="153" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>48</v>
       </c>
@@ -14059,7 +14062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>49</v>
       </c>
@@ -14163,7 +14166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>50</v>
       </c>
@@ -14267,7 +14270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>51</v>
       </c>
@@ -14276,7 +14279,7 @@
         <v>0.37410617419909442</v>
       </c>
     </row>
-    <row r="158" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>52</v>
       </c>
@@ -14285,7 +14288,7 @@
         <v>0.11643440731922046</v>
       </c>
     </row>
-    <row r="160" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>34</v>
       </c>
@@ -14389,7 +14392,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="161" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>53</v>
       </c>
@@ -14493,7 +14496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>54</v>
       </c>
@@ -14597,7 +14600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>55</v>
       </c>
@@ -14701,7 +14704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>56</v>
       </c>
@@ -14805,7 +14808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>57</v>
       </c>
@@ -14909,7 +14912,7 @@
         <v>113043000</v>
       </c>
     </row>
-    <row r="166" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>58</v>
       </c>
@@ -15013,7 +15016,7 @@
         <v>17631900</v>
       </c>
     </row>
-    <row r="167" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>59</v>
       </c>
@@ -15117,7 +15120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>60</v>
       </c>
@@ -15221,7 +15224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>61</v>
       </c>
@@ -15325,7 +15328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>62</v>
       </c>
@@ -15429,7 +15432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>63</v>
       </c>
@@ -15533,7 +15536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>64</v>
       </c>
@@ -15637,7 +15640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>65</v>
       </c>
@@ -15741,7 +15744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>66</v>
       </c>
@@ -15845,7 +15848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>67</v>
       </c>
@@ -15949,7 +15952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>68</v>
       </c>
@@ -16053,7 +16056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>69</v>
       </c>
@@ -16062,7 +16065,7 @@
         <v>5.6361071029368451E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>70</v>
       </c>
@@ -16071,7 +16074,7 @@
         <v>2.8245431637561897E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>71</v>
       </c>
@@ -16080,38 +16083,38 @@
         <v>4.9687560350897296E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="183" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="184" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="185" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="186" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="187" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="188" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="189" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="190" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="191" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="192" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="193" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="194" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="195" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="196" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="197" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="198" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="199" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="200" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="201" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B201" s="14"/>
     </row>
-    <row r="202" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="202" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B202" s="14"/>
     </row>
-    <row r="203" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="204" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="205" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="206" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="207" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="208" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="209" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="203" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="2:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B209" s="15"/>
       <c r="C209" s="15"/>
       <c r="D209" s="15"/>
@@ -16146,33 +16149,33 @@
       <c r="AG209" s="15"/>
       <c r="AH209" s="15"/>
     </row>
-    <row r="210" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="210" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AE210" s="15"/>
       <c r="AF210" s="15"/>
       <c r="AG210" s="15"/>
       <c r="AH210" s="15"/>
     </row>
-    <row r="211" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="212" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="213" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="214" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="215" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="216" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="217" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="218" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="219" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="220" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="221" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="222" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="211" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B222" s="16"/>
     </row>
-    <row r="223" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="223" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B223" s="16"/>
     </row>
-    <row r="224" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="224" spans="2:34" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B224" s="16"/>
     </row>
-    <row r="225" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="225" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -16180,22 +16183,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.9296875" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -16203,13 +16206,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2">
-        <f>Calibration!B4</f>
-        <v>2.95</v>
+        <f>Calibration!B4/10</f>
+        <v>0.29500000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>